<commit_message>
more clearance around vias
</commit_message>
<xml_diff>
--- a/isolation/bom.xlsx
+++ b/isolation/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/sb2919_ic_ac_uk/Documents/Uni/ICLR/Github/art-wally/isolation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="502" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA7EE05E-25C9-47E4-B60A-FD4FC8248B36}"/>
+  <xr:revisionPtr revIDLastSave="508" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EC665FB-635A-4721-9B13-C21BBA3B96D8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JLC" sheetId="1" r:id="rId1"/>
@@ -300,9 +300,6 @@
     <t>J1</t>
   </si>
   <si>
-    <t>JST-XH 4 pin</t>
-  </si>
-  <si>
     <t>J2</t>
   </si>
   <si>
@@ -682,6 +679,9 @@
   </si>
   <si>
     <t>C22</t>
+  </si>
+  <si>
+    <t>JST-PH 2 pin</t>
   </si>
 </sst>
 </file>
@@ -1355,7 +1355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -1381,7 +1381,7 @@
         <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -1407,7 +1407,7 @@
         <v>47</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>48</v>
@@ -1422,7 +1422,7 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M2" s="1">
         <f>SUM(Table1[Cost])</f>
@@ -1431,22 +1431,22 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="D3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>8</v>
@@ -1455,7 +1455,7 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M3" s="1">
         <f>Other!I2*1.25</f>
@@ -1464,16 +1464,16 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>58</v>
@@ -1488,7 +1488,7 @@
         <v>4.3E-3</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M4" s="1">
         <f>M2+M3</f>
@@ -1497,22 +1497,22 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="D5" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>8</v>
@@ -1523,16 +1523,16 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>58</v>
@@ -1549,22 +1549,22 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>8</v>
@@ -1575,16 +1575,16 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>58</v>
@@ -1601,16 +1601,16 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>44</v>
@@ -1627,16 +1627,16 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>44</v>
@@ -1653,16 +1653,16 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>44</v>
@@ -1679,16 +1679,16 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>44</v>
@@ -1714,7 +1714,7 @@
         <v>43</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>44</v>
@@ -1731,16 +1731,16 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>51</v>
@@ -1757,16 +1757,16 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>51</v>
@@ -1783,16 +1783,16 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>51</v>
@@ -1818,7 +1818,7 @@
         <v>57</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>58</v>
@@ -1844,7 +1844,7 @@
         <v>47</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>51</v>
@@ -1870,7 +1870,7 @@
         <v>47</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>51</v>
@@ -1896,7 +1896,7 @@
         <v>47</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>51</v>
@@ -1922,7 +1922,7 @@
         <v>47</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>51</v>
@@ -1939,22 +1939,22 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="D22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>8</v>
@@ -1965,16 +1965,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="D23" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>58</v>
@@ -2000,7 +2000,7 @@
         <v>16</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>17</v>
@@ -2017,22 +2017,22 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>8</v>
@@ -2043,22 +2043,22 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>8</v>
@@ -2069,22 +2069,22 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>8</v>
@@ -2104,7 +2104,7 @@
         <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>28</v>
@@ -2130,7 +2130,7 @@
         <v>11</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>6</v>
@@ -2147,22 +2147,22 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>8</v>
@@ -2173,22 +2173,22 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>8</v>
@@ -2199,22 +2199,22 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>8</v>
@@ -2225,22 +2225,22 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>8</v>
@@ -2251,22 +2251,22 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>8</v>
@@ -2286,7 +2286,7 @@
         <v>65</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>66</v>
@@ -2312,7 +2312,7 @@
         <v>76</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>73</v>
@@ -2329,7 +2329,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>62</v>
@@ -2338,7 +2338,7 @@
         <v>65</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>66</v>
@@ -2355,7 +2355,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>62</v>
@@ -2364,7 +2364,7 @@
         <v>76</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>73</v>
@@ -2381,22 +2381,22 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>8</v>
@@ -2407,22 +2407,22 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>8</v>
@@ -2433,22 +2433,22 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>8</v>
@@ -2459,22 +2459,22 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>8</v>
@@ -2494,7 +2494,7 @@
         <v>12</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>68</v>
@@ -2511,16 +2511,16 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="D44" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>36</v>
@@ -2537,16 +2537,16 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="D45" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>36</v>
@@ -2563,22 +2563,22 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>8</v>
@@ -2589,16 +2589,16 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>34</v>
@@ -2615,22 +2615,22 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>8</v>
@@ -2641,16 +2641,16 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>70</v>
@@ -2667,16 +2667,16 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>70</v>
@@ -2693,16 +2693,16 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>70</v>
@@ -2719,16 +2719,16 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>70</v>
@@ -2745,16 +2745,16 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>70</v>
@@ -2780,7 +2780,7 @@
         <v>32</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>34</v>
@@ -2797,16 +2797,16 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>70</v>
@@ -2823,16 +2823,16 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>70</v>
@@ -2849,16 +2849,16 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>70</v>
@@ -2875,16 +2875,16 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="D58" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>70</v>
@@ -2910,7 +2910,7 @@
         <v>33</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>36</v>
@@ -2936,7 +2936,7 @@
         <v>63</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>70</v>
@@ -2953,7 +2953,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>62</v>
@@ -2962,7 +2962,7 @@
         <v>63</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>70</v>
@@ -2988,7 +2988,7 @@
         <v>72</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>79</v>
@@ -3005,7 +3005,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>62</v>
@@ -3014,7 +3014,7 @@
         <v>72</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>79</v>
@@ -3031,16 +3031,16 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="D64" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>36</v>
@@ -3057,16 +3057,16 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="D65" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>36</v>
@@ -3094,8 +3094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EFD0D0-6010-4DE2-A740-5FED5A866A4A}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3177,7 +3177,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>60</v>
@@ -3203,10 +3203,10 @@
         <v>85</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>25</v>
@@ -3223,32 +3223,32 @@
         <v>60</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>87</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>87</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="C8" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>25</v>
@@ -3259,16 +3259,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>25</v>
@@ -3279,16 +3279,16 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>25</v>
@@ -3299,16 +3299,16 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>25</v>
@@ -3319,16 +3319,16 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>25</v>
@@ -3339,16 +3339,16 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>25</v>
@@ -3359,13 +3359,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>25</v>
@@ -3376,57 +3376,57 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wally ready for manufacture
</commit_message>
<xml_diff>
--- a/isolation/bom.xlsx
+++ b/isolation/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/sb2919_ic_ac_uk/Documents/Uni/ICLR/Github/art-wally/isolation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="539" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2ED5D75-255A-49C5-A21A-FC69522E9D8B}"/>
+  <xr:revisionPtr revIDLastSave="586" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9AB7186-D319-47F0-808B-E646D0A5A047}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JLC" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="212">
   <si>
     <t>PCB Ident</t>
   </si>
@@ -90,9 +90,6 @@
     <t>C22452</t>
   </si>
   <si>
-    <t>Subtotal</t>
-  </si>
-  <si>
     <t>IC1</t>
   </si>
   <si>
@@ -360,12 +357,6 @@
     <t>JLC Subtotal</t>
   </si>
   <si>
-    <t>Other Subtotal</t>
-  </si>
-  <si>
-    <t>Unit Subtotal</t>
-  </si>
-  <si>
     <t>IC5</t>
   </si>
   <si>
@@ -664,13 +655,31 @@
   </si>
   <si>
     <t>R09</t>
+  </si>
+  <si>
+    <t>Unit Cost</t>
+  </si>
+  <si>
+    <t>Components Total</t>
+  </si>
+  <si>
+    <t>Board Cost</t>
+  </si>
+  <si>
+    <t>Boards Required</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Board Subtotal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -705,6 +714,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -726,11 +741,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1069,7 +1085,7 @@
     <tableColumn id="3" xr3:uid="{CE48B791-2D4F-4219-9048-5825EE503154}" name="Name"/>
     <tableColumn id="4" xr3:uid="{35CE205C-CB5E-41F1-89C9-7410BA00354C}" name="Link" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{AA370C7A-B275-4F4A-8EBA-42D32DD66BEA}" name="Supplier" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{64BA8FDB-4E0C-4EE9-839D-D745472F8C6B}" name="Cost" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{64BA8FDB-4E0C-4EE9-839D-D745472F8C6B}" name="Unit Cost" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1340,33 +1356,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.54296875" style="1" customWidth="1"/>
-    <col min="3" max="4" width="20.81640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7265625" style="1" customWidth="1"/>
-    <col min="7" max="11" width="8.7265625" style="1"/>
-    <col min="12" max="12" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="2" width="11.5546875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="20.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" style="1" customWidth="1"/>
+    <col min="7" max="11" width="8.77734375" style="1"/>
+    <col min="12" max="12" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -1381,18 +1397,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>15</v>
@@ -1407,31 +1423,31 @@
         <v>4.2200000000000001E-2</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M2" s="1">
         <f>SUM(Table1[Cost])</f>
         <v>0.45180000000000009</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>7</v>
@@ -1439,32 +1455,25 @@
       <c r="H3" s="1">
         <v>1.7399999999999999E-2</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="M3" s="1">
-        <f>Other!I2*1.25</f>
-        <v>8.1649999999999991</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>7</v>
@@ -1472,32 +1481,25 @@
       <c r="H4" s="1">
         <v>1.7399999999999999E-2</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="M4" s="1">
-        <f>M2+M3</f>
-        <v>8.6167999999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>7</v>
@@ -1506,24 +1508,24 @@
         <v>1.7399999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>7</v>
@@ -1532,24 +1534,24 @@
         <v>1.7399999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>7</v>
@@ -1558,18 +1560,18 @@
         <v>1.7399999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>5</v>
@@ -1584,76 +1586,76 @@
         <v>1.5599999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="H9" s="1">
         <v>1.32E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="H10" s="1">
         <v>1.32E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>7</v>
@@ -1662,24 +1664,24 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>7</v>
@@ -1688,24 +1690,24 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>7</v>
@@ -1714,24 +1716,24 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>7</v>
@@ -1740,24 +1742,24 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>7</v>
@@ -1766,24 +1768,24 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>7</v>
@@ -1792,24 +1794,24 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>7</v>
@@ -1818,24 +1820,24 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>7</v>
@@ -1844,24 +1846,24 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>7</v>
@@ -1870,24 +1872,24 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>7</v>
@@ -1896,24 +1898,24 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>7</v>
@@ -1922,24 +1924,24 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>7</v>
@@ -1948,24 +1950,24 @@
         <v>9.7000000000000003E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>7</v>
@@ -1974,24 +1976,24 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>7</v>
@@ -2000,24 +2002,24 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>7</v>
@@ -2026,24 +2028,24 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>7</v>
@@ -2052,24 +2054,24 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>7</v>
@@ -2078,24 +2080,24 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>7</v>
@@ -2104,24 +2106,24 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>7</v>
@@ -2130,24 +2132,24 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>7</v>
@@ -2156,24 +2158,24 @@
         <v>6.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="E31" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>7</v>
@@ -2182,24 +2184,24 @@
         <v>6.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>7</v>
@@ -2208,24 +2210,24 @@
         <v>6.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>7</v>
@@ -2234,24 +2236,24 @@
         <v>5.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>7</v>
@@ -2260,24 +2262,24 @@
         <v>4.3E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="D35" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>7</v>
@@ -2286,24 +2288,24 @@
         <v>4.3E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="D36" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>7</v>
@@ -2312,24 +2314,24 @@
         <v>4.3E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="D37" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>7</v>
@@ -2338,24 +2340,24 @@
         <v>4.3E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>7</v>
@@ -2364,24 +2366,24 @@
         <v>4.3E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="D39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>7</v>
@@ -2390,24 +2392,24 @@
         <v>2.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="D40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>7</v>
@@ -2416,24 +2418,24 @@
         <v>2.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="D41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>7</v>
@@ -2442,24 +2444,24 @@
         <v>2.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>7</v>
@@ -2468,24 +2470,24 @@
         <v>2.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E43" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>7</v>
@@ -2494,24 +2496,24 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="D44" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E44" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>7</v>
@@ -2520,24 +2522,24 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="D45" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E45" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>7</v>
@@ -2546,24 +2548,24 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E46" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>7</v>
@@ -2572,24 +2574,24 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>7</v>
@@ -2598,24 +2600,24 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E48" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>7</v>
@@ -2624,24 +2626,24 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E49" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>7</v>
@@ -2650,24 +2652,24 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E50" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>7</v>
@@ -2676,24 +2678,24 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E51" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>7</v>
@@ -2702,24 +2704,24 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E52" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>7</v>
@@ -2728,24 +2730,24 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E53" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>7</v>
@@ -2754,24 +2756,24 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="D54" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E54" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>7</v>
@@ -2780,24 +2782,24 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E55" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>7</v>
@@ -2806,24 +2808,24 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E56" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>7</v>
@@ -2832,24 +2834,24 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E57" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F57" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>7</v>
@@ -2858,24 +2860,24 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E58" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>7</v>
@@ -2884,24 +2886,24 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>7</v>
@@ -2910,24 +2912,24 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E60" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>7</v>
@@ -2936,24 +2938,24 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E61" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>7</v>
@@ -2962,24 +2964,24 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E62" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>7</v>
@@ -2988,24 +2990,24 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="E63" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>7</v>
@@ -3014,24 +3016,24 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E64" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>7</v>
@@ -3040,24 +3042,24 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="E65" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>7</v>
@@ -3077,23 +3079,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EFD0D0-6010-4DE2-A740-5FED5A866A4A}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.90625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7265625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.1796875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="26.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.21875" style="1" customWidth="1"/>
+    <col min="6" max="10" width="8.77734375" style="1"/>
+    <col min="11" max="11" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3101,7 +3105,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>11</v>
@@ -3110,329 +3114,397 @@
         <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1">
         <v>1.2</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="1">
-        <f>SUM(Table13[Cost])</f>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="K2" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="L2" s="1">
+        <f>SUM(Table13[Unit Cost])</f>
         <v>6.532</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1">
         <v>0.88</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="K3" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="L3" s="1">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="1">
         <v>0.88</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="F6" s="1">
         <v>0.55200000000000005</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="K6" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="L6" s="1">
+        <f>+L2+L3</f>
+        <v>10.112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="1">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="K7" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="L7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="K8" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="L8" s="1">
+        <f>L6*L7</f>
+        <v>40.448</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="1">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="E10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" s="1">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12" s="1">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" s="1">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>177</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add two generic inputs to wally
had two gpio left lol
</commit_message>
<xml_diff>
--- a/isolation/bom.xlsx
+++ b/isolation/bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/sb2919_ic_ac_uk/Documents/Uni/ICLR/Github/art-wally/isolation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shrey\OneDrive - Imperial College London\Uni\ICLR\Github\art-wally\isolation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="602" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0D18F09-038E-4B43-99F4-7264A4523BAE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF726F5-0FEA-4116-A888-89E148C03CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JLC" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="216">
   <si>
     <t>PCB Ident</t>
   </si>
@@ -567,12 +567,6 @@
     <t>USB C Port</t>
   </si>
   <si>
-    <t>217175-0001</t>
-  </si>
-  <si>
-    <t>https://www.mouser.co.uk/ProductDetail/Molex/217175-0001?qs=DRkmTr78QARWJMiqNnldSg%3D%3D</t>
-  </si>
-  <si>
     <t>JST-PH 4 pin</t>
   </si>
   <si>
@@ -682,6 +676,15 @@
   </si>
   <si>
     <t>Boards Ordered</t>
+  </si>
+  <si>
+    <t>UJC-HP2-3-SMT-TR</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/CUI-Devices/UJC-HP2-3-SMT-TR?qs=HoCaDK9Nz5cglCCyoWNzZg%3D%3D</t>
+  </si>
+  <si>
+    <t>Added to order</t>
   </si>
 </sst>
 </file>
@@ -760,7 +763,25 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1063,38 +1084,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A0602E7-1A25-42E9-BF44-F09CA170C8FC}" name="Table1" displayName="Table1" ref="A1:H65" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A0602E7-1A25-42E9-BF44-F09CA170C8FC}" name="Table1" displayName="Table1" ref="A1:H65" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:H65" xr:uid="{2A0602E7-1A25-42E9-BF44-F09CA170C8FC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H65">
     <sortCondition descending="1" ref="H1:H65"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B4FAA6AB-83B4-4C84-8804-F1AC5BACE4BB}" name="PCB Ident" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{0CFD2752-679C-477B-B126-B8120AC92495}" name="Block" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{1B58CE16-B0B1-4054-B4AF-AABCB45AE617}" name="Description" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{7D3B067D-44F4-4C72-ADF9-31B9997A6B54}" name="Simple Name" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{B4FAA6AB-83B4-4C84-8804-F1AC5BACE4BB}" name="PCB Ident" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{0CFD2752-679C-477B-B126-B8120AC92495}" name="Block" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{1B58CE16-B0B1-4054-B4AF-AABCB45AE617}" name="Description" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{7D3B067D-44F4-4C72-ADF9-31B9997A6B54}" name="Simple Name" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{E962FE16-E8B6-45B0-A890-E5B3DFBB18B2}" name="JLC Name"/>
-    <tableColumn id="4" xr3:uid="{990A84E6-FEB3-4F0C-B071-D44C86705F1B}" name="JLC Code" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{D9AAA942-DED1-4B6A-855E-8BAC2D202809}" name="Basic" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{FF6A9334-BA71-474D-878B-F76ED55006AB}" name="Cost" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{990A84E6-FEB3-4F0C-B071-D44C86705F1B}" name="JLC Code" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{D9AAA942-DED1-4B6A-855E-8BAC2D202809}" name="Basic" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{FF6A9334-BA71-474D-878B-F76ED55006AB}" name="Cost" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF0408F7-95F1-4593-9198-21390B37E860}" name="Table13" displayName="Table13" ref="A1:F21" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:F21" xr:uid="{2A0602E7-1A25-42E9-BF44-F09CA170C8FC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF0408F7-95F1-4593-9198-21390B37E860}" name="Table13" displayName="Table13" ref="A1:G21" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:G21" xr:uid="{2A0602E7-1A25-42E9-BF44-F09CA170C8FC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F20">
     <sortCondition descending="1" ref="F1:F21"/>
   </sortState>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8119D89E-A3EC-4D25-9A33-22E21D26F7FD}" name="PCB Ident" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{F761C4B6-755A-4384-B088-D38BFCC162C6}" name="Desc" dataDxfId="3"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{8119D89E-A3EC-4D25-9A33-22E21D26F7FD}" name="PCB Ident" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{F761C4B6-755A-4384-B088-D38BFCC162C6}" name="Desc" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{CE48B791-2D4F-4219-9048-5825EE503154}" name="Name"/>
-    <tableColumn id="4" xr3:uid="{35CE205C-CB5E-41F1-89C9-7410BA00354C}" name="Link" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{AA370C7A-B275-4F4A-8EBA-42D32DD66BEA}" name="Supplier" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{64BA8FDB-4E0C-4EE9-839D-D745472F8C6B}" name="Unit Cost" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{35CE205C-CB5E-41F1-89C9-7410BA00354C}" name="Link" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{AA370C7A-B275-4F4A-8EBA-42D32DD66BEA}" name="Supplier" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{64BA8FDB-4E0C-4EE9-839D-D745472F8C6B}" name="Unit Cost" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{81EE38D3-4209-4742-BD68-9560901A265B}" name="Added to order" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1365,22 +1387,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="2" width="11.5546875" style="1" customWidth="1"/>
-    <col min="3" max="4" width="20.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" style="1" customWidth="1"/>
-    <col min="7" max="11" width="8.77734375" style="1"/>
-    <col min="12" max="12" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="2" width="11.53125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="20.796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.53125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.796875" style="1" customWidth="1"/>
+    <col min="7" max="11" width="8.796875" style="1"/>
+    <col min="12" max="12" width="11.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1406,7 +1428,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1439,9 +1461,9 @@
         <v>0.45180000000000009</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>35</v>
@@ -1465,7 +1487,7 @@
         <v>1.7399999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>166</v>
       </c>
@@ -1491,14 +1513,14 @@
         <v>1.7399999999999999E-2</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M4" s="1">
         <f>21.8+15.47</f>
         <v>37.270000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>167</v>
       </c>
@@ -1524,14 +1546,14 @@
         <v>1.7399999999999999E-2</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="M5" s="1">
         <f>(M4*1.2)/1.25</f>
         <v>35.779200000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>168</v>
       </c>
@@ -1557,7 +1579,7 @@
         <v>1.7399999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>169</v>
       </c>
@@ -1583,15 +1605,15 @@
         <v>1.7399999999999999E-2</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="M7" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>36</v>
@@ -1615,16 +1637,16 @@
         <v>1.5599999999999999E-2</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M8" s="1">
         <f>M5/M7</f>
         <v>3.5779200000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>49</v>
@@ -1648,9 +1670,9 @@
         <v>1.32E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>49</v>
@@ -1674,9 +1696,9 @@
         <v>1.32E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>136</v>
@@ -1700,9 +1722,9 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>136</v>
@@ -1726,9 +1748,9 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>136</v>
@@ -1752,9 +1774,9 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>136</v>
@@ -1778,7 +1800,7 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>141</v>
       </c>
@@ -1804,7 +1826,7 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>142</v>
       </c>
@@ -1830,7 +1852,7 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>143</v>
       </c>
@@ -1856,7 +1878,7 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>144</v>
       </c>
@@ -1882,7 +1904,7 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>145</v>
       </c>
@@ -1908,9 +1930,9 @@
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>49</v>
@@ -1934,9 +1956,9 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>49</v>
@@ -1960,7 +1982,7 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -1986,9 +2008,9 @@
         <v>9.7000000000000003E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>35</v>
@@ -2012,9 +2034,9 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>35</v>
@@ -2038,9 +2060,9 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>35</v>
@@ -2064,9 +2086,9 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>35</v>
@@ -2090,7 +2112,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
         <v>171</v>
       </c>
@@ -2116,7 +2138,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
         <v>172</v>
       </c>
@@ -2142,7 +2164,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
         <v>173</v>
       </c>
@@ -2168,7 +2190,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
         <v>126</v>
       </c>
@@ -2194,7 +2216,7 @@
         <v>6.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
         <v>127</v>
       </c>
@@ -2220,7 +2242,7 @@
         <v>6.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
         <v>128</v>
       </c>
@@ -2246,9 +2268,9 @@
         <v>6.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>35</v>
@@ -2272,9 +2294,9 @@
         <v>5.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>35</v>
@@ -2298,9 +2320,9 @@
         <v>4.3E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>73</v>
@@ -2324,7 +2346,7 @@
         <v>4.3E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
         <v>95</v>
       </c>
@@ -2350,7 +2372,7 @@
         <v>4.3E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
         <v>104</v>
       </c>
@@ -2376,7 +2398,7 @@
         <v>4.3E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A38" s="1" t="s">
         <v>134</v>
       </c>
@@ -2402,9 +2424,9 @@
         <v>4.3E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>73</v>
@@ -2428,7 +2450,7 @@
         <v>2.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A40" s="1" t="s">
         <v>96</v>
       </c>
@@ -2454,7 +2476,7 @@
         <v>2.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A41" s="1" t="s">
         <v>103</v>
       </c>
@@ -2480,7 +2502,7 @@
         <v>2.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A42" s="1" t="s">
         <v>133</v>
       </c>
@@ -2506,9 +2528,9 @@
         <v>2.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A43" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>36</v>
@@ -2532,9 +2554,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A44" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>49</v>
@@ -2558,9 +2580,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A45" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>49</v>
@@ -2584,9 +2606,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>49</v>
@@ -2610,9 +2632,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A47" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>49</v>
@@ -2636,7 +2658,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A48" s="1" t="s">
         <v>146</v>
       </c>
@@ -2662,7 +2684,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A49" s="1" t="s">
         <v>147</v>
       </c>
@@ -2688,7 +2710,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A50" s="1" t="s">
         <v>148</v>
       </c>
@@ -2714,7 +2736,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A51" s="1" t="s">
         <v>149</v>
       </c>
@@ -2740,7 +2762,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A52" s="1" t="s">
         <v>150</v>
       </c>
@@ -2766,7 +2788,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A53" s="1" t="s">
         <v>151</v>
       </c>
@@ -2792,7 +2814,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A54" s="1" t="s">
         <v>152</v>
       </c>
@@ -2818,7 +2840,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A55" s="1" t="s">
         <v>153</v>
       </c>
@@ -2844,7 +2866,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A56" s="1" t="s">
         <v>154</v>
       </c>
@@ -2870,9 +2892,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A57" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>35</v>
@@ -2896,9 +2918,9 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A58" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>35</v>
@@ -2922,9 +2944,9 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A59" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>114</v>
@@ -2948,9 +2970,9 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A60" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>114</v>
@@ -2974,7 +2996,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A61" s="1" t="s">
         <v>77</v>
       </c>
@@ -3000,7 +3022,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A62" s="1" t="s">
         <v>113</v>
       </c>
@@ -3026,7 +3048,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A63" s="1" t="s">
         <v>78</v>
       </c>
@@ -3052,7 +3074,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A64" s="1" t="s">
         <v>119</v>
       </c>
@@ -3078,7 +3100,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A65" s="1" t="s">
         <v>120</v>
       </c>
@@ -3117,23 +3139,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29EFD0D0-6010-4DE2-A740-5FED5A866A4A}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.53125" style="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.21875" style="1" customWidth="1"/>
-    <col min="6" max="10" width="8.77734375" style="1"/>
-    <col min="11" max="11" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.77734375" style="1"/>
+    <col min="3" max="3" width="26.86328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.19921875" style="1" customWidth="1"/>
+    <col min="6" max="10" width="8.796875" style="1"/>
+    <col min="11" max="11" width="18.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3150,10 +3172,13 @@
         <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="B2" s="1" t="s">
         <v>116</v>
       </c>
@@ -3169,17 +3194,19 @@
       <c r="F2" s="1">
         <v>1.2</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="H2" s="4"/>
       <c r="K2" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="L2" s="1">
         <f>SUM(Table13[Unit Cost])</f>
-        <v>6.532</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <v>6.3460000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>65</v>
       </c>
@@ -3198,17 +3225,19 @@
       <c r="F3" s="1">
         <v>0.88</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="H3" s="4"/>
       <c r="K3" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L3" s="1">
         <f>JLC!M8</f>
         <v>3.5779200000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>72</v>
       </c>
@@ -3227,10 +3256,12 @@
       <c r="F4" s="1">
         <v>0.88</v>
       </c>
-      <c r="G4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>121</v>
       </c>
@@ -3238,21 +3269,23 @@
         <v>175</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>176</v>
+        <v>213</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>177</v>
+        <v>214</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="1">
-        <v>0.65</v>
-      </c>
-      <c r="G5" s="4"/>
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -3271,17 +3304,19 @@
       <c r="F6" s="1">
         <v>0.55200000000000005</v>
       </c>
-      <c r="G6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="H6" s="4"/>
       <c r="K6" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L6" s="1">
         <f>+L2+L3</f>
-        <v>10.109920000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+        <v>9.9239200000000007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>106</v>
       </c>
@@ -3300,16 +3335,18 @@
       <c r="F7" s="1">
         <v>0.37</v>
       </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="K7" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="L7" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>107</v>
       </c>
@@ -3328,17 +3365,19 @@
       <c r="F8" s="1">
         <v>0.37</v>
       </c>
-      <c r="G8" s="4"/>
+      <c r="G8" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="K8" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="L8" s="1">
         <f>L6*L7</f>
-        <v>60.659520000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>59.543520000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>108</v>
       </c>
@@ -3357,10 +3396,12 @@
       <c r="F9" s="1">
         <v>0.37</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>109</v>
       </c>
@@ -3379,10 +3420,12 @@
       <c r="F10" s="1">
         <v>0.37</v>
       </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>97</v>
       </c>
@@ -3401,10 +3444,12 @@
       <c r="F11" s="1">
         <v>0.32</v>
       </c>
-      <c r="G11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>68</v>
       </c>
@@ -3423,10 +3468,12 @@
       <c r="F12" s="1">
         <v>0.31</v>
       </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>99</v>
       </c>
@@ -3445,10 +3492,12 @@
       <c r="F13" s="1">
         <v>0.26</v>
       </c>
-      <c r="G13" s="4"/>
+      <c r="G13" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>70</v>
       </c>
@@ -3456,12 +3505,12 @@
         <v>48</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>71</v>
       </c>
@@ -3469,12 +3518,12 @@
         <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>156</v>
       </c>
@@ -3487,7 +3536,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>157</v>
       </c>
@@ -3500,7 +3549,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>158</v>
       </c>
@@ -3513,7 +3562,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>160</v>
       </c>
@@ -3526,7 +3575,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>161</v>
       </c>
@@ -3539,7 +3588,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>

</xml_diff>